<commit_message>
Commot reserve core flow
</commit_message>
<xml_diff>
--- a/document/function/FunctionList.xlsx
+++ b/document/function/FunctionList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MinhQuy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CapstoneProject\SWP49X-FFRS\document\function\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
   <si>
     <t>Function List</t>
   </si>
@@ -258,13 +258,50 @@
   </si>
   <si>
     <t>/swp49x-ffrs/time-enable/field-owner-and-type</t>
+  </si>
+  <si>
+    <t>Get Free Time</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/match/free-time</t>
+  </si>
+  <si>
+    <t>field-owner-id, field-type-id, date</t>
+  </si>
+  <si>
+    <t>List&lt;TimeSlotEntity&gt;</t>
+  </si>
+  <si>
+    <t>Reserve Friendly Match</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/match/friendly-match</t>
+  </si>
+  <si>
+    <t>InputReservationDTO</t>
+  </si>
+  <si>
+    <t>FriendlyMatchEntity</t>
+  </si>
+  <si>
+    <t>Get Match Up Coming</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/match/upcoming-match</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,7 +386,9 @@
       <right style="thin">
         <color theme="0"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -359,13 +398,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,27 +727,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1192,27 +1232,27 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+      <c r="A21" s="7">
         <v>19</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
+      <c r="E21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1320,24 +1360,99 @@
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="7" t="s">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit get 10 Account Entity And Search Account Entity By Name
</commit_message>
<xml_diff>
--- a/document/function/FunctionList.xlsx
+++ b/document/function/FunctionList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
   <si>
     <t>Function List</t>
   </si>
@@ -360,6 +360,24 @@
   </si>
   <si>
     <t>TourMatchEntity</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/account/top-10-field-owner</t>
+  </si>
+  <si>
+    <t>Get Top 10 Field Owner Nearest</t>
+  </si>
+  <si>
+    <t>longitude, latitude</t>
+  </si>
+  <si>
+    <t>Find Account Entity Have Name Like And Role</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/account/name</t>
+  </si>
+  <si>
+    <t>name, role</t>
   </si>
 </sst>
 </file>
@@ -468,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -478,12 +496,41 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFFEE2EF"/>
@@ -800,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,52 +1104,52 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>29</v>
+      <c r="B11" s="3"/>
+      <c r="C11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1112,72 +1159,72 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>29</v>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1187,23 +1234,23 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>44</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1212,17 +1259,17 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>44</v>
@@ -1237,145 +1284,145 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="I20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
+      <c r="E22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>19</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
+      <c r="I22" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
+      <c r="E23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1385,23 +1432,23 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
         <v>63</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1410,10 +1457,10 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>18</v>
@@ -1423,85 +1470,85 @@
         <v>13</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
-        <v>24</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="I26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8" t="s">
+      <c r="F28" s="8"/>
+      <c r="G28" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>29</v>
+      <c r="I28" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1510,10 +1557,10 @@
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>18</v>
@@ -1535,23 +1582,23 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>88</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1560,20 +1607,20 @@
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>30</v>
@@ -1585,23 +1632,23 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1610,23 +1657,23 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G33" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="H33" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1635,23 +1682,23 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1660,10 +1707,10 @@
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>9</v>
@@ -1671,11 +1718,9 @@
       <c r="F35" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="G35" s="4"/>
       <c r="H35" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>29</v>
@@ -1687,22 +1732,74 @@
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit update from master
</commit_message>
<xml_diff>
--- a/document/function/FunctionList.xlsx
+++ b/document/function/FunctionList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
   <si>
     <t>Function List</t>
   </si>
@@ -360,6 +360,24 @@
   </si>
   <si>
     <t>TourMatchEntity</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/account/top-10-field-owner</t>
+  </si>
+  <si>
+    <t>Get Top 10 Field Owner Nearest</t>
+  </si>
+  <si>
+    <t>longitude, latitude</t>
+  </si>
+  <si>
+    <t>Find Account Entity Have Name Like And Role</t>
+  </si>
+  <si>
+    <t>/swp49x-ffrs/account/name</t>
+  </si>
+  <si>
+    <t>name, role</t>
   </si>
 </sst>
 </file>
@@ -468,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -478,12 +496,41 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFFEE2EF"/>
@@ -800,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,52 +1104,52 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>29</v>
+      <c r="B11" s="3"/>
+      <c r="C11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1112,72 +1159,72 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>29</v>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1187,23 +1234,23 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>44</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1212,17 +1259,17 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>44</v>
@@ -1237,145 +1284,145 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="I20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
+      <c r="E22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>19</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
+      <c r="I22" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
+      <c r="E23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1385,23 +1432,23 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
         <v>63</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1410,10 +1457,10 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>18</v>
@@ -1423,85 +1470,85 @@
         <v>13</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
-        <v>24</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="I26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8" t="s">
+      <c r="F28" s="8"/>
+      <c r="G28" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>29</v>
+      <c r="I28" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1510,10 +1557,10 @@
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>18</v>
@@ -1535,23 +1582,23 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>88</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1560,20 +1607,20 @@
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>30</v>
@@ -1585,23 +1632,23 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1610,23 +1657,23 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G33" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="H33" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1635,23 +1682,23 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1660,10 +1707,10 @@
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>9</v>
@@ -1671,11 +1718,9 @@
       <c r="F35" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="G35" s="4"/>
       <c r="H35" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>29</v>
@@ -1687,22 +1732,74 @@
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>